<commit_message>
first pass at code to redistribute all garbage codes in a big loop
</commit_message>
<xml_diff>
--- a/data/cod/raw/GC/garbageRedistribution.xlsx
+++ b/data/cod/raw/GC/garbageRedistribution.xlsx
@@ -94,9 +94,9 @@
       <sheetName val="ICD9 to USCOD for stata"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="1">
           <cell r="A1" t="str">
@@ -435,9 +435,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1175,7 +1175,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12:G13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,33 +1291,33 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>USCOD!B33</f>
-        <v>G_1</v>
+        <f>USCOD!B34</f>
+        <v>G_2</v>
       </c>
       <c r="B2" t="str">
-        <f>USCOD!A33</f>
-        <v>Septicaemia</v>
+        <f>USCOD!A34</f>
+        <v>Heart Failure</v>
       </c>
       <c r="C2" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -1341,13 +1341,13 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
@@ -1373,15 +1373,15 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>USCOD!B34</f>
-        <v>G_2</v>
+        <f>USCOD!B38</f>
+        <v>G_6</v>
       </c>
       <c r="B3" t="str">
-        <f>USCOD!A34</f>
-        <v>Heart Failure</v>
+        <f>USCOD!A38</f>
+        <v>Ill-Defined Cardio</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1426,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="R3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="1">
         <v>1</v>
@@ -1537,508 +1537,508 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
+        <f>USCOD!B41</f>
+        <v>G_9</v>
+      </c>
+      <c r="B5" t="str">
+        <f>USCOD!A41</f>
+        <v>Undetermined Intent</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>USCOD!B40</f>
+        <v>G_8</v>
+      </c>
+      <c r="B6" t="str">
+        <f>USCOD!A40</f>
+        <v>Ill-Defined Injury</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>USCOD!B42</f>
+        <v>G_10</v>
+      </c>
+      <c r="B7" t="str">
+        <f>USCOD!A42</f>
+        <v>Ill-Defined Infectious</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>USCOD!B33</f>
+        <v>G_1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>USCOD!A33</f>
+        <v>Septicaemia</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
         <f>USCOD!B36</f>
         <v>G_4</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B9" t="str">
         <f>USCOD!A36</f>
         <v>Volume Depletion</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C9" s="1">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0</v>
-      </c>
-      <c r="V5" s="1">
-        <v>0</v>
-      </c>
-      <c r="W5" s="1">
-        <v>1</v>
-      </c>
-      <c r="X5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>1</v>
+      </c>
+      <c r="X9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>USCOD!B39</f>
+        <v>G_7</v>
+      </c>
+      <c r="B10" t="str">
+        <f>USCOD!A39</f>
+        <v>Renal Failure</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="1">
+        <v>1</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
         <f>USCOD!B37</f>
         <v>G_5</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B11" t="str">
         <f>USCOD!A37</f>
         <v>Ill-Defined</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1">
-        <v>1</v>
-      </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1</v>
-      </c>
-      <c r="V6" s="1">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1">
-        <v>1</v>
-      </c>
-      <c r="X6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>USCOD!B38</f>
-        <v>G_6</v>
-      </c>
-      <c r="B7" t="str">
-        <f>USCOD!A38</f>
-        <v>Ill-Defined Cardio</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>1</v>
-      </c>
-      <c r="R7" s="1">
-        <v>1</v>
-      </c>
-      <c r="S7" s="1">
-        <v>1</v>
-      </c>
-      <c r="T7" s="1">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1">
-        <v>0</v>
-      </c>
-      <c r="V7" s="1">
-        <v>0</v>
-      </c>
-      <c r="W7" s="1">
-        <v>0</v>
-      </c>
-      <c r="X7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>USCOD!B39</f>
-        <v>G_7</v>
-      </c>
-      <c r="B8" t="str">
-        <f>USCOD!A39</f>
-        <v>Renal Failure</v>
-      </c>
-      <c r="C8" s="1">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0</v>
-      </c>
-      <c r="S8" s="1">
-        <v>1</v>
-      </c>
-      <c r="T8" s="1">
-        <v>0</v>
-      </c>
-      <c r="U8" s="1">
-        <v>0</v>
-      </c>
-      <c r="V8" s="1">
-        <v>1</v>
-      </c>
-      <c r="W8" s="1">
-        <v>0</v>
-      </c>
-      <c r="X8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>USCOD!B40</f>
-        <v>G_8</v>
-      </c>
-      <c r="B9" t="str">
-        <f>USCOD!A40</f>
-        <v>Ill-Defined Injury</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1">
-        <v>0</v>
-      </c>
-      <c r="T9" s="1">
-        <v>0</v>
-      </c>
-      <c r="U9" s="1">
-        <v>0</v>
-      </c>
-      <c r="V9" s="1">
-        <v>0</v>
-      </c>
-      <c r="W9" s="1">
-        <v>1</v>
-      </c>
-      <c r="X9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>USCOD!B41</f>
-        <v>G_9</v>
-      </c>
-      <c r="B10" t="str">
-        <f>USCOD!A41</f>
-        <v>Undetermined Intent</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>0</v>
-      </c>
-      <c r="R10" s="1">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1">
-        <v>0</v>
-      </c>
-      <c r="T10" s="1">
-        <v>0</v>
-      </c>
-      <c r="U10" s="1">
-        <v>0</v>
-      </c>
-      <c r="V10" s="1">
-        <v>0</v>
-      </c>
-      <c r="W10" s="1">
-        <v>0</v>
-      </c>
-      <c r="X10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>USCOD!B42</f>
-        <v>G_10</v>
-      </c>
-      <c r="B11" t="str">
-        <f>USCOD!A42</f>
-        <v>Ill-Defined Infectious</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
-      </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -2058,58 +2058,61 @@
         <v>1</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:Z11">
+    <sortCondition ref="C2:C11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed maternal/perinatal from ill-defined infectious targets
</commit_message>
<xml_diff>
--- a/data/cod/raw/GC/garbageRedistribution.xlsx
+++ b/data/cod/raw/GC/garbageRedistribution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10800" windowHeight="10155" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="10800" windowHeight="10095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="USCOD" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,7 +1175,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,10 +1718,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
added some basic priors to the logistic redistribution model to account for really strong beliefs - e.g. that ill-defined cancers should be redistributed onto cancer; updated garbage redistribution worksheet to reflect these (which are still much more general than the proportional redistribution method)
</commit_message>
<xml_diff>
--- a/data/cod/raw/GC/garbageRedistribution.xlsx
+++ b/data/cod/raw/GC/garbageRedistribution.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Description</t>
   </si>
@@ -26,7 +26,31 @@
     <t>GC</t>
   </si>
   <si>
-    <t>Order</t>
+    <t>Ill-Defined Cancer</t>
+  </si>
+  <si>
+    <t>Ill-Defined Injury</t>
+  </si>
+  <si>
+    <t>Undetermined Intent</t>
+  </si>
+  <si>
+    <t>Heart Failure</t>
+  </si>
+  <si>
+    <t>Ill-Defined Infectious</t>
+  </si>
+  <si>
+    <t>Volume Depletion</t>
+  </si>
+  <si>
+    <t>Ill-Defined Cardio</t>
+  </si>
+  <si>
+    <t>Ill-Defined</t>
+  </si>
+  <si>
+    <t>Septicaemia</t>
   </si>
 </sst>
 </file>
@@ -284,7 +308,7 @@
         </row>
         <row r="24">
           <cell r="A24" t="str">
-            <v>Other NCDs</v>
+            <v>Renal Failure</v>
           </cell>
           <cell r="B24" t="str">
             <v>B_6</v>
@@ -292,122 +316,122 @@
         </row>
         <row r="25">
           <cell r="A25" t="str">
-            <v>Injuries</v>
+            <v>Other NCDs</v>
           </cell>
           <cell r="B25" t="str">
-            <v>C</v>
+            <v>B_7</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26" t="str">
-            <v>Unintentional Injuries</v>
+            <v>Injuries</v>
           </cell>
           <cell r="B26" t="str">
-            <v>C_1</v>
+            <v>C</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27" t="str">
-            <v>RTI</v>
+            <v>Unintentional Injuries</v>
           </cell>
           <cell r="B27" t="str">
-            <v>C_1_1</v>
+            <v>C_1</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28" t="str">
-            <v>Other Unintentional Injuries</v>
+            <v>RTI</v>
           </cell>
           <cell r="B28" t="str">
-            <v>C_1_2</v>
+            <v>C_1_1</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29" t="str">
-            <v>Intentional Injuries</v>
+            <v>Other Unintentional Injuries</v>
           </cell>
           <cell r="B29" t="str">
-            <v>C_2</v>
+            <v>C_1_2</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30" t="str">
-            <v>Suicide</v>
+            <v>Intentional Injuries</v>
           </cell>
           <cell r="B30" t="str">
-            <v>C_2_1</v>
+            <v>C_2</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>Homicide/War</v>
+            <v>Suicide</v>
           </cell>
           <cell r="B31" t="str">
-            <v>C_2_2</v>
+            <v>C_2_1</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32" t="str">
-            <v>Garbage</v>
+            <v>Homicide/War</v>
           </cell>
           <cell r="B32" t="str">
-            <v>G</v>
+            <v>C_2_2</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33" t="str">
-            <v>Septicaemia</v>
+            <v>Garbage</v>
           </cell>
           <cell r="B33" t="str">
-            <v>G_1</v>
+            <v>G</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34" t="str">
-            <v>Heart Failure</v>
+            <v>Septicaemia</v>
           </cell>
           <cell r="B34" t="str">
-            <v>G_2</v>
+            <v>G_1</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35" t="str">
-            <v>Ill-Defined Cancer</v>
+            <v>Heart Failure</v>
           </cell>
           <cell r="B35" t="str">
-            <v>G_3</v>
+            <v>G_2</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36" t="str">
-            <v>Volume Depletion</v>
+            <v>Ill-Defined Cancer</v>
           </cell>
           <cell r="B36" t="str">
-            <v>G_4</v>
+            <v>G_3</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37" t="str">
-            <v>Ill-Defined</v>
+            <v>Volume Depletion</v>
           </cell>
           <cell r="B37" t="str">
-            <v>G_5</v>
+            <v>G_4</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38" t="str">
-            <v>Ill-Defined Cardio</v>
+            <v>Ill-Defined</v>
           </cell>
           <cell r="B38" t="str">
-            <v>G_6</v>
+            <v>G_5</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39" t="str">
-            <v>Renal Failure</v>
+            <v>Ill-Defined Cardio</v>
           </cell>
           <cell r="B39" t="str">
-            <v>G_7</v>
+            <v>G_6</v>
           </cell>
         </row>
         <row r="40">
@@ -415,7 +439,7 @@
             <v>Ill-Defined Injury</v>
           </cell>
           <cell r="B40" t="str">
-            <v>G_8</v>
+            <v>G_7</v>
           </cell>
         </row>
         <row r="41">
@@ -423,7 +447,7 @@
             <v>Undetermined Intent</v>
           </cell>
           <cell r="B41" t="str">
-            <v>G_9</v>
+            <v>G_8</v>
           </cell>
         </row>
         <row r="42">
@@ -431,7 +455,7 @@
             <v>Ill-Defined Infectious</v>
           </cell>
           <cell r="B42" t="str">
-            <v>G_10</v>
+            <v>G_9</v>
           </cell>
         </row>
       </sheetData>
@@ -734,7 +758,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,7 +999,7 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>[1]USCOD!A24</f>
-        <v>Other NCDs</v>
+        <v>Renal Failure</v>
       </c>
       <c r="B24" t="str">
         <f>[1]USCOD!B24</f>
@@ -985,151 +1009,151 @@
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>[1]USCOD!A25</f>
-        <v>Injuries</v>
+        <v>Other NCDs</v>
       </c>
       <c r="B25" t="str">
         <f>[1]USCOD!B25</f>
-        <v>C</v>
+        <v>B_7</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>[1]USCOD!A26</f>
-        <v>Unintentional Injuries</v>
+        <v>Injuries</v>
       </c>
       <c r="B26" t="str">
         <f>[1]USCOD!B26</f>
-        <v>C_1</v>
+        <v>C</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>[1]USCOD!A27</f>
-        <v>RTI</v>
+        <v>Unintentional Injuries</v>
       </c>
       <c r="B27" t="str">
         <f>[1]USCOD!B27</f>
-        <v>C_1_1</v>
+        <v>C_1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>[1]USCOD!A28</f>
-        <v>Other Unintentional Injuries</v>
+        <v>RTI</v>
       </c>
       <c r="B28" t="str">
         <f>[1]USCOD!B28</f>
-        <v>C_1_2</v>
+        <v>C_1_1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>[1]USCOD!A29</f>
-        <v>Intentional Injuries</v>
+        <v>Other Unintentional Injuries</v>
       </c>
       <c r="B29" t="str">
         <f>[1]USCOD!B29</f>
-        <v>C_2</v>
+        <v>C_1_2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>[1]USCOD!A30</f>
-        <v>Suicide</v>
+        <v>Intentional Injuries</v>
       </c>
       <c r="B30" t="str">
         <f>[1]USCOD!B30</f>
-        <v>C_2_1</v>
+        <v>C_2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>[1]USCOD!A31</f>
-        <v>Homicide/War</v>
+        <v>Suicide</v>
       </c>
       <c r="B31" t="str">
         <f>[1]USCOD!B31</f>
-        <v>C_2_2</v>
+        <v>C_2_1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>[1]USCOD!A32</f>
-        <v>Garbage</v>
+        <v>Homicide/War</v>
       </c>
       <c r="B32" t="str">
         <f>[1]USCOD!B32</f>
-        <v>G</v>
+        <v>C_2_2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>[1]USCOD!A33</f>
-        <v>Septicaemia</v>
+        <v>Garbage</v>
       </c>
       <c r="B33" t="str">
         <f>[1]USCOD!B33</f>
-        <v>G_1</v>
+        <v>G</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>[1]USCOD!A34</f>
-        <v>Heart Failure</v>
+        <v>Septicaemia</v>
       </c>
       <c r="B34" t="str">
         <f>[1]USCOD!B34</f>
-        <v>G_2</v>
+        <v>G_1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>[1]USCOD!A35</f>
-        <v>Ill-Defined Cancer</v>
+        <v>Heart Failure</v>
       </c>
       <c r="B35" t="str">
         <f>[1]USCOD!B35</f>
-        <v>G_3</v>
+        <v>G_2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>[1]USCOD!A36</f>
-        <v>Volume Depletion</v>
+        <v>Ill-Defined Cancer</v>
       </c>
       <c r="B36" t="str">
         <f>[1]USCOD!B36</f>
-        <v>G_4</v>
+        <v>G_3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>[1]USCOD!A37</f>
-        <v>Ill-Defined</v>
+        <v>Volume Depletion</v>
       </c>
       <c r="B37" t="str">
         <f>[1]USCOD!B37</f>
-        <v>G_5</v>
+        <v>G_4</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>[1]USCOD!A38</f>
-        <v>Ill-Defined Cardio</v>
+        <v>Ill-Defined</v>
       </c>
       <c r="B38" t="str">
         <f>[1]USCOD!B38</f>
-        <v>G_6</v>
+        <v>G_5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>[1]USCOD!A39</f>
-        <v>Renal Failure</v>
+        <v>Ill-Defined Cardio</v>
       </c>
       <c r="B39" t="str">
         <f>[1]USCOD!B39</f>
-        <v>G_7</v>
+        <v>G_6</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1139,7 +1163,7 @@
       </c>
       <c r="B40" t="str">
         <f>[1]USCOD!B40</f>
-        <v>G_8</v>
+        <v>G_7</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1149,7 +1173,7 @@
       </c>
       <c r="B41" t="str">
         <f>[1]USCOD!B41</f>
-        <v>G_9</v>
+        <v>G_8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1183,7 @@
       </c>
       <c r="B42" t="str">
         <f>[1]USCOD!B42</f>
-        <v>G_10</v>
+        <v>G_9</v>
       </c>
     </row>
   </sheetData>
@@ -1169,21 +1193,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="1" customWidth="1"/>
-    <col min="4" max="26" width="5.85546875" customWidth="1"/>
+    <col min="3" max="26" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -1193,195 +1216,194 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="str">
+      <c r="C1" s="1" t="str">
         <f>USCOD!$B3</f>
         <v>A_1</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="D1" s="1" t="str">
         <f>USCOD!$B4</f>
         <v>A_2</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="E1" s="1" t="str">
         <f>USCOD!$B5</f>
         <v>A_3</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="F1" s="1" t="str">
         <f>USCOD!$B6</f>
         <v>A_4</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="G1" s="1" t="str">
         <f>USCOD!$B7</f>
         <v>A_5</v>
       </c>
-      <c r="I1" s="1" t="str">
+      <c r="H1" s="1" t="str">
         <f>USCOD!$B8</f>
         <v>A_6</v>
       </c>
-      <c r="J1" s="1" t="str">
+      <c r="I1" s="1" t="str">
         <f>USCOD!$B11</f>
         <v>B_1_1</v>
       </c>
-      <c r="K1" s="1" t="str">
+      <c r="J1" s="1" t="str">
         <f>USCOD!$B12</f>
         <v>B_1_2</v>
       </c>
-      <c r="L1" s="1" t="str">
+      <c r="K1" s="1" t="str">
         <f>USCOD!$B13</f>
         <v>B_1_3</v>
       </c>
-      <c r="M1" s="1" t="str">
+      <c r="L1" s="1" t="str">
         <f>USCOD!$B14</f>
         <v>B_1_4</v>
       </c>
-      <c r="N1" s="1" t="str">
+      <c r="M1" s="1" t="str">
         <f>USCOD!$B15</f>
         <v>B_1_5</v>
       </c>
-      <c r="O1" s="1" t="str">
+      <c r="N1" s="1" t="str">
         <f>USCOD!$B16</f>
         <v>B_1_6</v>
       </c>
-      <c r="P1" s="1" t="str">
+      <c r="O1" s="1" t="str">
         <f>USCOD!$B17</f>
         <v>B_2</v>
       </c>
-      <c r="Q1" s="1" t="str">
+      <c r="P1" s="1" t="str">
         <f>USCOD!$B19</f>
         <v>B_3_1</v>
       </c>
-      <c r="R1" s="1" t="str">
+      <c r="Q1" s="1" t="str">
         <f>USCOD!$B20</f>
         <v>B_3_2</v>
       </c>
-      <c r="S1" s="1" t="str">
+      <c r="R1" s="1" t="str">
         <f>USCOD!$B21</f>
         <v>B_3_3</v>
       </c>
-      <c r="T1" s="1" t="str">
+      <c r="S1" s="1" t="str">
         <f>USCOD!$B22</f>
         <v>B_4</v>
       </c>
-      <c r="U1" s="1" t="str">
+      <c r="T1" s="1" t="str">
         <f>USCOD!$B23</f>
         <v>B_5</v>
       </c>
-      <c r="V1" s="1" t="str">
+      <c r="U1" s="1" t="str">
         <f>USCOD!$B24</f>
         <v>B_6</v>
       </c>
+      <c r="V1" s="1" t="str">
+        <f>USCOD!$B25</f>
+        <v>B_7</v>
+      </c>
       <c r="W1" s="1" t="str">
-        <f>USCOD!$B27</f>
+        <f>USCOD!$B28</f>
         <v>C_1_1</v>
       </c>
       <c r="X1" s="1" t="str">
-        <f>USCOD!$B28</f>
+        <f>USCOD!$B29</f>
         <v>C_1_2</v>
       </c>
       <c r="Y1" s="1" t="str">
-        <f>USCOD!$B30</f>
+        <f>USCOD!$B31</f>
         <v>C_2_1</v>
       </c>
       <c r="Z1" s="1" t="str">
-        <f>USCOD!$B31</f>
+        <f>USCOD!$B32</f>
         <v>C_2_2</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>USCOD!B34</f>
-        <v>G_2</v>
-      </c>
-      <c r="B2" t="str">
-        <f>USCOD!A34</f>
-        <v>Heart Failure</v>
+        <f>VLOOKUP(B2,USCOD!A:B,2,FALSE)</f>
+        <v>G_1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
       </c>
       <c r="R2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="1">
         <v>1</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>USCOD!B38</f>
-        <v>G_6</v>
-      </c>
-      <c r="B3" t="str">
-        <f>USCOD!A38</f>
-        <v>Ill-Defined Cardio</v>
+        <f>VLOOKUP(B3,USCOD!A:B,2,FALSE)</f>
+        <v>G_2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1417,10 +1439,10 @@
         <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
@@ -1432,13 +1454,13 @@
         <v>1</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="1">
         <v>0</v>
@@ -1455,15 +1477,14 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>USCOD!B35</f>
+        <f>VLOOKUP(B4,USCOD!A:B,2,FALSE)</f>
         <v>G_3</v>
       </c>
-      <c r="B4" t="str">
-        <f>USCOD!A35</f>
-        <v>Ill-Defined Cancer</v>
+      <c r="B4" t="s">
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -1481,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -1499,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
@@ -1537,75 +1558,74 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>USCOD!B41</f>
-        <v>G_9</v>
-      </c>
-      <c r="B5" t="str">
-        <f>USCOD!A41</f>
-        <v>Undetermined Intent</v>
+        <f>VLOOKUP(B5,USCOD!A:B,2,FALSE)</f>
+        <v>G_4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" s="1">
         <v>1</v>
@@ -1619,72 +1639,71 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>USCOD!B40</f>
-        <v>G_8</v>
-      </c>
-      <c r="B6" t="str">
-        <f>USCOD!A40</f>
-        <v>Ill-Defined Injury</v>
+        <f>VLOOKUP(B6,USCOD!A:B,2,FALSE)</f>
+        <v>G_5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="1">
         <v>1</v>
@@ -1693,29 +1712,28 @@
         <v>1</v>
       </c>
       <c r="Y6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>USCOD!B42</f>
-        <v>G_10</v>
-      </c>
-      <c r="B7" t="str">
-        <f>USCOD!A42</f>
-        <v>Ill-Defined Infectious</v>
+        <f>VLOOKUP(B7,USCOD!A:B,2,FALSE)</f>
+        <v>G_6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1724,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -1745,28 +1763,28 @@
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="1">
         <v>0</v>
@@ -1783,33 +1801,32 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>USCOD!B33</f>
-        <v>G_1</v>
-      </c>
-      <c r="B8" t="str">
-        <f>USCOD!A33</f>
-        <v>Septicaemia</v>
+        <f>VLOOKUP(B8,USCOD!A:B,2,FALSE)</f>
+        <v>G_7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
@@ -1851,29 +1868,28 @@
         <v>0</v>
       </c>
       <c r="W8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>USCOD!B36</f>
-        <v>G_4</v>
-      </c>
-      <c r="B9" t="str">
-        <f>USCOD!A36</f>
-        <v>Volume Depletion</v>
+        <f>VLOOKUP(B9,USCOD!A:B,2,FALSE)</f>
+        <v>G_8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -1888,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -1933,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="W9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9" s="1">
         <v>1</v>
@@ -1947,30 +1963,29 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>USCOD!B39</f>
-        <v>G_7</v>
-      </c>
-      <c r="B10" t="str">
-        <f>USCOD!A39</f>
-        <v>Renal Failure</v>
+        <f>VLOOKUP(B10,USCOD!A:B,2,FALSE)</f>
+        <v>G_9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
       </c>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
@@ -1994,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="1">
         <v>0</v>
@@ -2003,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="1">
         <v>0</v>
@@ -2012,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="1">
         <v>0</v>
@@ -2027,92 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>USCOD!B37</f>
-        <v>G_5</v>
-      </c>
-      <c r="B11" t="str">
-        <f>USCOD!A37</f>
-        <v>Ill-Defined</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1</v>
-      </c>
-      <c r="O11" s="1">
-        <v>1</v>
-      </c>
-      <c r="P11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1">
-        <v>1</v>
-      </c>
-      <c r="S11" s="1">
-        <v>1</v>
-      </c>
-      <c r="T11" s="1">
-        <v>1</v>
-      </c>
-      <c r="U11" s="1">
-        <v>1</v>
-      </c>
-      <c r="V11" s="1">
-        <v>1</v>
-      </c>
-      <c r="W11" s="1">
-        <v>1</v>
-      </c>
-      <c r="X11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:Z11">
-    <sortCondition ref="C2:C11"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>